<commit_message>
Milestone 4 blog update - Pradheep
</commit_message>
<xml_diff>
--- a/blog Milestone 4.xlsx
+++ b/blog Milestone 4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\github\Library-Management-System-COEN-6312\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pradheep\Desktop\Library-Management-System-COEN-6312\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCCCA4A-4D0C-41A4-A400-4E9DAB68CBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD567B62-FDD2-425F-820A-B355F58187E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="237">
   <si>
     <t>Team Members</t>
   </si>
@@ -711,6 +711,39 @@
   </si>
   <si>
     <t>Implementation of the OCL table</t>
+  </si>
+  <si>
+    <t>UML diagrams</t>
+  </si>
+  <si>
+    <t>Sequence Diagram</t>
+  </si>
+  <si>
+    <t>Free user buys membership</t>
+  </si>
+  <si>
+    <t>Paid user Fns</t>
+  </si>
+  <si>
+    <t>Rework on Paid user Mng</t>
+  </si>
+  <si>
+    <t>Communication diagrams</t>
+  </si>
+  <si>
+    <t>Comm diag for membership</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Format reworking UML</t>
+  </si>
+  <si>
+    <t>Formating and Captioning</t>
+  </si>
+  <si>
+    <t>Format report</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1218,6 +1251,19 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1549,10 +1595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S145"/>
+  <dimension ref="A1:S152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="70" workbookViewId="0">
-      <selection activeCell="K115" sqref="K115"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="70" workbookViewId="0">
+      <selection activeCell="T145" sqref="T145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1575,13 +1621,13 @@
     <row r="1" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H3" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="57"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="55"/>
-      <c r="S3" s="60" t="s">
+      <c r="H3" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="60"/>
+      <c r="S3" s="65" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1589,8 +1635,8 @@
       <c r="H4" s="1"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="59"/>
-      <c r="S4" s="61"/>
+      <c r="K4" s="64"/>
+      <c r="S4" s="66"/>
     </row>
     <row r="5" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H5" s="4" t="s">
@@ -1602,8 +1648,8 @@
       <c r="J5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="59"/>
-      <c r="S5" s="61"/>
+      <c r="K5" s="64"/>
+      <c r="S5" s="66"/>
     </row>
     <row r="6" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H6" s="7" t="s">
@@ -1616,7 +1662,7 @@
         <v>7</v>
       </c>
       <c r="K6" s="9"/>
-      <c r="S6" s="61"/>
+      <c r="S6" s="66"/>
     </row>
     <row r="7" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H7" s="7" t="s">
@@ -1629,7 +1675,7 @@
         <v>10</v>
       </c>
       <c r="K7" s="9"/>
-      <c r="S7" s="61"/>
+      <c r="S7" s="66"/>
     </row>
     <row r="8" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H8" s="7" t="s">
@@ -1642,7 +1688,7 @@
         <v>11</v>
       </c>
       <c r="K8" s="9"/>
-      <c r="S8" s="61"/>
+      <c r="S8" s="66"/>
     </row>
     <row r="9" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H9" s="7" t="s">
@@ -1655,7 +1701,7 @@
         <v>15</v>
       </c>
       <c r="K9" s="9"/>
-      <c r="S9" s="61"/>
+      <c r="S9" s="66"/>
     </row>
     <row r="10" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H10" s="7" t="s">
@@ -1668,7 +1714,7 @@
         <v>18</v>
       </c>
       <c r="K10" s="9"/>
-      <c r="S10" s="61"/>
+      <c r="S10" s="66"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="10" t="s">
@@ -1681,7 +1727,7 @@
         <v>21</v>
       </c>
       <c r="K11" s="12"/>
-      <c r="S11" s="61"/>
+      <c r="S11" s="66"/>
     </row>
     <row r="12" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="S12" t="s">
@@ -1695,41 +1741,41 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="51"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="56"/>
       <c r="G15" s="13"/>
-      <c r="H15" s="54" t="s">
+      <c r="H15" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="55" t="s">
+      <c r="I15" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="54" t="s">
+      <c r="J15" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="54" t="s">
+      <c r="K15" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="L15" s="49" t="s">
+      <c r="L15" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="50"/>
-      <c r="P15" s="51"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="55"/>
+      <c r="P15" s="56"/>
       <c r="Q15" s="14"/>
       <c r="R15" s="15"/>
     </row>
     <row r="16" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="53"/>
+      <c r="A16" s="58"/>
       <c r="B16" s="16" t="str">
         <f>$J$6</f>
         <v>Sai</v>
@@ -1754,10 +1800,10 @@
         <f>$J$11</f>
         <v>AS</v>
       </c>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
       <c r="L16" s="16" t="str">
         <f>$J$6</f>
         <v>Sai</v>
@@ -7170,87 +7216,148 @@
         <v>0</v>
       </c>
       <c r="R134" s="17">
-        <f>SUM(L141:P141)</f>
+        <f>SUM(L148:P148)</f>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="35"/>
+      <c r="A135" s="49">
+        <v>45378</v>
+      </c>
       <c r="B135" s="33"/>
       <c r="C135" s="33"/>
       <c r="D135" s="33"/>
-      <c r="E135" s="33"/>
+      <c r="E135" s="33">
+        <v>1</v>
+      </c>
       <c r="F135" s="33"/>
       <c r="G135" s="33"/>
-      <c r="H135" s="33"/>
-      <c r="I135" s="36"/>
-      <c r="J135" s="33"/>
-      <c r="K135" s="34"/>
-      <c r="L135" s="30"/>
-      <c r="M135" s="30"/>
-      <c r="N135" s="30"/>
-      <c r="O135" s="30"/>
-      <c r="P135" s="25"/>
-      <c r="Q135" s="25"/>
-      <c r="R135" s="17"/>
+      <c r="H135" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="I135" s="36">
+        <v>1.5</v>
+      </c>
+      <c r="J135" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="K135" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="L135" s="50"/>
+      <c r="M135" s="50"/>
+      <c r="N135" s="50"/>
+      <c r="O135" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="P135" s="51"/>
+      <c r="Q135" s="51"/>
+      <c r="R135" s="43"/>
     </row>
     <row r="136" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="29"/>
-      <c r="H136" s="30"/>
-      <c r="K136" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="L136">
-        <f t="shared" ref="L136:Q136" si="97">SUM(L134:L135)</f>
-        <v>0</v>
-      </c>
-      <c r="M136">
-        <f t="shared" si="97"/>
-        <v>0</v>
-      </c>
-      <c r="N136">
-        <f t="shared" si="97"/>
-        <v>0</v>
-      </c>
-      <c r="O136">
-        <f t="shared" si="97"/>
-        <v>0</v>
-      </c>
-      <c r="P136" s="17">
-        <f t="shared" si="97"/>
-        <v>0</v>
-      </c>
-      <c r="Q136" s="17">
-        <f t="shared" si="97"/>
-        <v>0</v>
-      </c>
+      <c r="A136" s="49">
+        <v>45383</v>
+      </c>
+      <c r="B136" s="33"/>
+      <c r="C136" s="33"/>
+      <c r="D136" s="33"/>
+      <c r="E136" s="33">
+        <v>1</v>
+      </c>
+      <c r="F136" s="33"/>
+      <c r="G136" s="33"/>
+      <c r="H136" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="I136" s="36">
+        <v>1</v>
+      </c>
+      <c r="J136" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="K136" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="L136" s="30"/>
+      <c r="M136" s="30"/>
+      <c r="N136" s="30"/>
+      <c r="O136" s="30">
+        <v>1</v>
+      </c>
+      <c r="P136" s="25"/>
+      <c r="Q136" s="25"/>
       <c r="R136" s="17"/>
     </row>
     <row r="137" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="29"/>
-      <c r="K137" t="s">
-        <v>203</v>
-      </c>
-      <c r="P137" s="17"/>
-      <c r="Q137" s="31"/>
-      <c r="R137" s="17">
-        <f>SUM(L136:Q136)</f>
-        <v>0</v>
-      </c>
+      <c r="A137" s="52">
+        <v>45384</v>
+      </c>
+      <c r="B137" s="33"/>
+      <c r="C137" s="33"/>
+      <c r="D137" s="33"/>
+      <c r="E137" s="33">
+        <v>1</v>
+      </c>
+      <c r="F137" s="33"/>
+      <c r="G137" s="33"/>
+      <c r="H137" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="I137" s="36">
+        <v>2</v>
+      </c>
+      <c r="J137" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="K137" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="L137" s="30"/>
+      <c r="M137" s="30"/>
+      <c r="N137" s="30"/>
+      <c r="O137" s="30">
+        <v>2</v>
+      </c>
+      <c r="P137" s="51"/>
+      <c r="Q137" s="51"/>
+      <c r="R137" s="43"/>
     </row>
     <row r="138" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="29" t="s">
-        <v>204</v>
-      </c>
-      <c r="L138" s="23"/>
-      <c r="M138" s="19"/>
-      <c r="N138" s="19"/>
-      <c r="O138" s="19"/>
-      <c r="P138" s="24"/>
-      <c r="Q138" s="25"/>
+      <c r="A138" s="49">
+        <v>45385</v>
+      </c>
+      <c r="B138" s="33"/>
+      <c r="C138" s="33"/>
+      <c r="D138" s="33"/>
+      <c r="E138" s="33">
+        <v>1</v>
+      </c>
+      <c r="F138" s="33"/>
+      <c r="G138" s="33"/>
+      <c r="H138" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="I138" s="36">
+        <v>2</v>
+      </c>
+      <c r="J138" s="33" t="s">
+        <v>231</v>
+      </c>
+      <c r="K138" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="L138" s="30"/>
+      <c r="M138" s="30"/>
+      <c r="N138" s="30"/>
+      <c r="O138" s="30">
+        <v>2</v>
+      </c>
+      <c r="P138" s="51"/>
+      <c r="Q138" s="51"/>
+      <c r="R138" s="43"/>
     </row>
     <row r="139" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="35"/>
+      <c r="A139" s="49"/>
       <c r="B139" s="33"/>
       <c r="C139" s="33"/>
       <c r="D139" s="33"/>
@@ -7261,33 +7368,16 @@
       <c r="I139" s="36"/>
       <c r="J139" s="33"/>
       <c r="K139" s="34"/>
-      <c r="L139" s="32">
-        <f t="shared" ref="L139:Q139" si="98">B139*$I139</f>
-        <v>0</v>
-      </c>
-      <c r="M139" s="37">
-        <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
-      <c r="N139" s="37">
-        <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
-      <c r="O139" s="37">
-        <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
-      <c r="P139" s="38">
-        <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
-      <c r="Q139" s="38">
-        <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
+      <c r="L139" s="30"/>
+      <c r="M139" s="30"/>
+      <c r="N139" s="30"/>
+      <c r="O139" s="30"/>
+      <c r="P139" s="51"/>
+      <c r="Q139" s="51"/>
+      <c r="R139" s="43"/>
     </row>
     <row r="140" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="35"/>
+      <c r="A140" s="49"/>
       <c r="B140" s="33"/>
       <c r="C140" s="33"/>
       <c r="D140" s="33"/>
@@ -7302,103 +7392,283 @@
       <c r="M140" s="30"/>
       <c r="N140" s="30"/>
       <c r="O140" s="30"/>
-      <c r="P140" s="25"/>
-      <c r="Q140" s="25"/>
+      <c r="P140" s="51"/>
+      <c r="Q140" s="51"/>
+      <c r="R140" s="43"/>
     </row>
     <row r="141" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="29"/>
-      <c r="H141" s="30"/>
-      <c r="K141" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="L141">
-        <f t="shared" ref="L141:Q141" si="99">SUM(L139:L140)</f>
-        <v>0</v>
-      </c>
-      <c r="M141">
-        <f t="shared" si="99"/>
-        <v>0</v>
-      </c>
-      <c r="N141">
-        <f t="shared" si="99"/>
-        <v>0</v>
-      </c>
-      <c r="O141">
-        <f t="shared" si="99"/>
-        <v>0</v>
-      </c>
-      <c r="P141" s="17">
-        <f t="shared" si="99"/>
-        <v>0</v>
-      </c>
-      <c r="Q141" s="17">
-        <f t="shared" si="99"/>
-        <v>0</v>
-      </c>
+      <c r="A141" s="49">
+        <v>45389</v>
+      </c>
+      <c r="B141" s="33"/>
+      <c r="C141" s="33"/>
+      <c r="D141" s="33"/>
+      <c r="E141" s="33">
+        <v>1</v>
+      </c>
+      <c r="F141" s="33"/>
+      <c r="G141" s="33"/>
+      <c r="H141" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="I141" s="36">
+        <v>2.5</v>
+      </c>
+      <c r="J141" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="K141" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="L141" s="30"/>
+      <c r="M141" s="30"/>
+      <c r="N141" s="30"/>
+      <c r="O141" s="30">
+        <v>3</v>
+      </c>
+      <c r="P141" s="51"/>
+      <c r="Q141" s="51"/>
+      <c r="R141" s="43"/>
     </row>
     <row r="142" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="29"/>
-      <c r="K142" t="s">
-        <v>205</v>
-      </c>
-      <c r="P142" s="17"/>
-      <c r="Q142" s="17"/>
+      <c r="A142" s="53">
+        <v>45389</v>
+      </c>
+      <c r="B142" s="33"/>
+      <c r="C142" s="33"/>
+      <c r="D142" s="33"/>
+      <c r="E142" s="33">
+        <v>1</v>
+      </c>
+      <c r="F142" s="33"/>
+      <c r="G142" s="33"/>
+      <c r="H142" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="I142" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="J142" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="K142" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="L142" s="30"/>
+      <c r="M142" s="30"/>
+      <c r="N142" s="30"/>
+      <c r="O142" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="P142" s="50"/>
+      <c r="Q142" s="50"/>
+      <c r="R142" s="43"/>
     </row>
     <row r="143" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="29"/>
-      <c r="P143" s="17"/>
-      <c r="Q143" s="17"/>
+      <c r="H143" s="30"/>
+      <c r="K143" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="L143">
+        <f>SUM(L134:L136)</f>
+        <v>0</v>
+      </c>
+      <c r="M143">
+        <f>SUM(M134:M136)</f>
+        <v>0</v>
+      </c>
+      <c r="N143">
+        <f>SUM(N134:N136)</f>
+        <v>0</v>
+      </c>
+      <c r="O143">
+        <f>SUM(O134:O142)</f>
+        <v>10</v>
+      </c>
+      <c r="P143" s="17">
+        <f>SUM(P134:P136)</f>
+        <v>0</v>
+      </c>
+      <c r="Q143" s="17">
+        <f>SUM(Q134:Q136)</f>
+        <v>0</v>
+      </c>
+      <c r="R143" s="17"/>
     </row>
     <row r="144" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="29"/>
-      <c r="K144" s="39" t="s">
+      <c r="K144" t="s">
+        <v>203</v>
+      </c>
+      <c r="P144" s="17"/>
+      <c r="Q144" s="31"/>
+      <c r="R144" s="17">
+        <f>SUM(L143:Q143)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="L145" s="23"/>
+      <c r="M145" s="19"/>
+      <c r="N145" s="19"/>
+      <c r="O145" s="19"/>
+      <c r="P145" s="24"/>
+      <c r="Q145" s="25"/>
+    </row>
+    <row r="146" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="35"/>
+      <c r="B146" s="33"/>
+      <c r="C146" s="33"/>
+      <c r="D146" s="33"/>
+      <c r="E146" s="33"/>
+      <c r="F146" s="33"/>
+      <c r="G146" s="33"/>
+      <c r="H146" s="33"/>
+      <c r="I146" s="36"/>
+      <c r="J146" s="33"/>
+      <c r="K146" s="34"/>
+      <c r="L146" s="32">
+        <f t="shared" ref="L146:Q146" si="97">B146*$I146</f>
+        <v>0</v>
+      </c>
+      <c r="M146" s="37">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="N146" s="37">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="O146" s="37">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="P146" s="38">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="Q146" s="38">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="35"/>
+      <c r="B147" s="33"/>
+      <c r="C147" s="33"/>
+      <c r="D147" s="33"/>
+      <c r="E147" s="33"/>
+      <c r="F147" s="33"/>
+      <c r="G147" s="33"/>
+      <c r="H147" s="33"/>
+      <c r="I147" s="36"/>
+      <c r="J147" s="33"/>
+      <c r="K147" s="34"/>
+      <c r="L147" s="30"/>
+      <c r="M147" s="30"/>
+      <c r="N147" s="30"/>
+      <c r="O147" s="30"/>
+      <c r="P147" s="25"/>
+      <c r="Q147" s="25"/>
+    </row>
+    <row r="148" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="29"/>
+      <c r="H148" s="30"/>
+      <c r="K148" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="L148">
+        <f t="shared" ref="L148:Q148" si="98">SUM(L146:L147)</f>
+        <v>0</v>
+      </c>
+      <c r="M148">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="N148">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="O148">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="P148" s="17">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="Q148" s="17">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="29"/>
+      <c r="K149" t="s">
+        <v>205</v>
+      </c>
+      <c r="P149" s="17"/>
+      <c r="Q149" s="17"/>
+    </row>
+    <row r="150" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="29"/>
+      <c r="P150" s="17"/>
+      <c r="Q150" s="17"/>
+    </row>
+    <row r="151" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="29"/>
+      <c r="K151" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="L144">
-        <f t="shared" ref="L144:Q144" si="100">L34+L90+L130+L136+L141</f>
+      <c r="L151">
+        <f t="shared" ref="L151:Q151" si="99">L34+L90+L130+L143+L148</f>
         <v>68.5</v>
       </c>
-      <c r="M144">
-        <f t="shared" si="100"/>
+      <c r="M151">
+        <f t="shared" si="99"/>
         <v>69.5</v>
       </c>
-      <c r="N144">
-        <f t="shared" si="100"/>
+      <c r="N151">
+        <f t="shared" si="99"/>
         <v>70.5</v>
       </c>
-      <c r="O144">
-        <f t="shared" si="100"/>
-        <v>72</v>
-      </c>
-      <c r="P144" s="17">
-        <f t="shared" si="100"/>
+      <c r="O151">
+        <f t="shared" si="99"/>
+        <v>82</v>
+      </c>
+      <c r="P151" s="17">
+        <f t="shared" si="99"/>
         <v>71</v>
       </c>
-      <c r="Q144" s="17">
-        <f t="shared" si="100"/>
+      <c r="Q151" s="17">
+        <f t="shared" si="99"/>
         <v>68.5</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="40"/>
-      <c r="B145" s="41"/>
-      <c r="C145" s="41"/>
-      <c r="D145" s="41"/>
-      <c r="E145" s="41"/>
-      <c r="F145" s="41"/>
-      <c r="G145" s="41"/>
-      <c r="H145" s="41"/>
-      <c r="I145" s="41"/>
-      <c r="J145" s="41"/>
-      <c r="K145" s="42" t="s">
+    <row r="152" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="40"/>
+      <c r="B152" s="41"/>
+      <c r="C152" s="41"/>
+      <c r="D152" s="41"/>
+      <c r="E152" s="41"/>
+      <c r="F152" s="41"/>
+      <c r="G152" s="41"/>
+      <c r="H152" s="41"/>
+      <c r="I152" s="41"/>
+      <c r="J152" s="41"/>
+      <c r="K152" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="L145" s="41"/>
-      <c r="M145" s="41"/>
-      <c r="N145" s="41"/>
-      <c r="O145" s="41"/>
-      <c r="P145" s="31"/>
-      <c r="Q145" s="31"/>
+      <c r="L152" s="41"/>
+      <c r="M152" s="41"/>
+      <c r="N152" s="41"/>
+      <c r="O152" s="41"/>
+      <c r="P152" s="31"/>
+      <c r="Q152" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>